<commit_message>
Updates to NA Param file column and row names
</commit_message>
<xml_diff>
--- a/parameters/NA/ammonia/country_parameters.xlsx
+++ b/parameters/NA/ammonia/country_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samiyhanaqvi/Desktop/SHIELD/restructuring_and_integration/GeoX/parameters/NA/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samiyhanaqvi/Desktop/SHIELD/updating-main/Geo-X/parameters/NA/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215664B3-469C-FA4B-B7D0-ECB66FED6082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8474F934-7433-2443-8FA0-F097ED4C25A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1560" windowWidth="28800" windowHeight="15340" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Country</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Namibia</t>
+  </si>
+  <si>
+    <t>Hydro interest rate</t>
+  </si>
+  <si>
+    <t>Hydro lifetime (years)</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,11 +444,11 @@
     <col min="6" max="6" width="26.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" customWidth="1"/>
     <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,19 +471,25 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -499,16 +511,16 @@
       <c r="G2">
         <v>20</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.10881498793561939</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>20</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>6.8154093053735251E-2</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing geothermal and ammonia issue, and time period of weather data and demand schedule
</commit_message>
<xml_diff>
--- a/parameters/NA/ammonia/country_parameters.xlsx
+++ b/parameters/NA/ammonia/country_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samiyhanaqvi/Desktop/SHIELD/updating-main/Geo-X/parameters/NA/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samiyhanaqvi/Desktop/SHIELD/adding-geothermal-main/Geo-X/parameters/NA/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8474F934-7433-2443-8FA0-F097ED4C25A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4016F243-F189-5441-8ABB-6527C1A4F86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1560" windowWidth="28800" windowHeight="15340" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="29080" windowHeight="18060" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Country</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Hydro lifetime (years)</t>
+  </si>
+  <si>
+    <t>Geothermal interest rate</t>
+  </si>
+  <si>
+    <t>Geothermal lifetime (years)</t>
   </si>
 </sst>
 </file>
@@ -428,27 +434,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,19 +486,25 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -511,6 +526,12 @@
       <c r="G2">
         <v>20</v>
       </c>
+      <c r="H2">
+        <v>0.10881498793561939</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
       <c r="J2">
         <v>0.10881498793561939</v>
       </c>
@@ -518,9 +539,15 @@
         <v>20</v>
       </c>
       <c r="L2">
+        <v>0.10881498793561939</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
         <v>6.8154093053735251E-2</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>50</v>
       </c>
     </row>

</xml_diff>